<commit_message>
Adjust GB per month cost for network components
</commit_message>
<xml_diff>
--- a/Configuration.Management.xlsx
+++ b/Configuration.Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://harveynashvn-my.sharepoint.com/personal/vietvuh1_nashtechglobal_com/Documents/Documents/Projects/AWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="11_F25DC773A252ABDACC1048FA499C5AAE5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EB271CD-BA30-426E-9877-0A94C493777A}"/>
+  <xr:revisionPtr revIDLastSave="570" documentId="11_F25DC773A252ABDACC1048FA499C5AAE5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EC9BC58-4A2D-439A-B3D8-2C438774D96F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -42,76 +42,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Viet Vu Hoang</author>
-  </authors>
-  <commentList>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{E0C75AA9-1419-4132-9932-531CBC878CDE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Viet Vu Hoang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-10GB per Month
-0.14GB per hour</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Viet Vu Hoang</author>
-  </authors>
-  <commentList>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{B73157AB-0A2A-4526-A1F8-9C848A52DBEF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Viet Vu Hoang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-10GB per Month
-0.14GB per hour</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -135,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -290,9 +220,6 @@
     <t>Number of Ips</t>
   </si>
   <si>
-    <t>GB</t>
-  </si>
-  <si>
     <t>Dev</t>
   </si>
   <si>
@@ -507,13 +434,31 @@
   </si>
   <si>
     <t>Monthly Cost</t>
+  </si>
+  <si>
+    <t>GB month</t>
+  </si>
+  <si>
+    <t>Year to Months</t>
+  </si>
+  <si>
+    <t>3 Years to Months</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>Yearly Cost</t>
+  </si>
+  <si>
+    <t>3 years Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,19 +473,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -571,6 +503,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -621,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -632,15 +571,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,12 +893,12 @@
         <v>35</v>
       </c>
       <c r="B2">
-        <f>SUM(Dev.Compoments!H6:H92)</f>
-        <v>1848.732</v>
+        <f>SUM(Dev.Compoments!H5:H91)</f>
+        <v>1850.1480000000001</v>
       </c>
       <c r="C2">
-        <f>SUM(Dev.Compoments!G6:G92)</f>
-        <v>199.46699999999998</v>
+        <f>SUM(Dev.Compoments!G5:G91)</f>
+        <v>199.58499999999998</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,12 +906,12 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <f>SUM(Prod.Compoments!G5:G93)</f>
-        <v>3661.3296</v>
+        <f>SUM(Prod.Compoments!G7:G95)</f>
+        <v>3610.212</v>
       </c>
       <c r="C3">
-        <f>SUM(Prod.Compoments!H5:H93)</f>
-        <v>9091.8287999999993</v>
+        <f>SUM(Prod.Compoments!H7:H95)</f>
+        <v>8938.4759999999987</v>
       </c>
     </row>
   </sheetData>
@@ -980,11 +920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF4B207-4132-4B4B-9A98-5F4F7A31A4FE}">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF4B207-4132-4B4B-9A98-5F4F7A31A4FE}">
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +945,7 @@
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="8"/>
     </row>
@@ -1024,142 +964,164 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="10">
-        <f>SUM(G7:G101)</f>
-        <v>199.46699999999998</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="10">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6">
-        <f>C4/Time.Units!$B$2</f>
-        <v>4.10958904109589E-3</v>
+        <f>SUM(G6:G100)</f>
+        <v>199.58499999999998</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>33</v>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" ref="D6">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))</f>
+        <v>Number of VPC</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f>$C$2</f>
+        <v>ap-southeast-1</v>
+      </c>
+      <c r="G6" cm="1">
+        <f t="array" ref="G6">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))*E6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" cm="1">
+        <f t="array" ref="H6">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))*E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))*E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" ref="D7">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))</f>
-        <v>Number of VPC</v>
+        <v>Number of Instances</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="str">
-        <f>$C$2</f>
+        <f t="shared" ref="F7:F10" si="0">$C$2</f>
         <v>ap-southeast-1</v>
       </c>
       <c r="G7" cm="1">
         <f t="array" ref="G7">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))*E7</f>
-        <v>0</v>
+        <v>43.07</v>
       </c>
       <c r="H7" cm="1">
         <f t="array" ref="H7">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))*E7</f>
-        <v>0</v>
+        <v>516.83999999999992</v>
       </c>
       <c r="I7" cm="1">
         <f t="array" ref="I7">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))*E7</f>
-        <v>0</v>
+        <v>1550.52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" ref="D8">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))</f>
-        <v>Number of Instances</v>
+        <v>GB month</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" ref="F8:F11" si="0">$C$2</f>
+        <f t="shared" si="0"/>
         <v>ap-southeast-1</v>
       </c>
       <c r="G8" cm="1">
         <f t="array" ref="G8">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))*E8</f>
-        <v>43.07</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="H8" cm="1">
         <f t="array" ref="H8">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))*E8</f>
-        <v>516.83999999999992</v>
+        <v>3.54</v>
       </c>
       <c r="I8" cm="1">
         <f t="array" ref="I8">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))*E8</f>
-        <v>1550.52</v>
+        <v>10.619999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" ref="D9">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))</f>
-        <v>GB</v>
+        <v>Number of Ips</v>
       </c>
       <c r="E9">
-        <f>D4</f>
-        <v>4.10958904109589E-3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -1167,30 +1129,30 @@
       </c>
       <c r="G9" cm="1">
         <f t="array" ref="G9">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))*E9</f>
-        <v>0.17699999999999999</v>
+        <v>7.3</v>
       </c>
       <c r="H9" cm="1">
         <f t="array" ref="H9">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))*E9</f>
-        <v>2.1239999999999997</v>
+        <v>87.600000000000009</v>
       </c>
       <c r="I9" cm="1">
         <f t="array" ref="I9">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))*E9</f>
-        <v>6.371999999999999</v>
+        <v>262.8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" ref="D10">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))</f>
-        <v>Number of Ips</v>
+        <v>Number of Instances</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1201,54 +1163,37 @@
       </c>
       <c r="G10" cm="1">
         <f t="array" ref="G10">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))*E10</f>
-        <v>7.3</v>
+        <v>148.91999999999999</v>
       </c>
       <c r="H10" cm="1">
         <f t="array" ref="H10">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))*E10</f>
-        <v>87.600000000000009</v>
+        <v>1242.1680000000001</v>
       </c>
       <c r="I10" cm="1">
         <f t="array" ref="I10">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))*E10</f>
-        <v>262.8</v>
+        <v>2465.0639999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="str" cm="1">
-        <f t="array" ref="D11">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))</f>
-        <v>Number of Instances</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>ap-southeast-1</v>
+        <v>6</v>
       </c>
       <c r="G11" cm="1">
         <f t="array" ref="G11">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))*E11</f>
-        <v>148.91999999999999</v>
+        <v>0</v>
       </c>
       <c r="H11" cm="1">
         <f t="array" ref="H11">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))*E11</f>
-        <v>1242.1680000000001</v>
+        <v>0</v>
       </c>
       <c r="I11" cm="1">
         <f t="array" ref="I11">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))*E11</f>
-        <v>2465.0639999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G12" cm="1">
         <f t="array" ref="G12">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C12)*(Pricing!E:E=F12), 0))*E12</f>
@@ -1265,7 +1210,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13" cm="1">
         <f t="array" ref="G13">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C13)*(Pricing!E:E=F13), 0))*E13</f>
@@ -1282,7 +1227,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" cm="1">
         <f t="array" ref="G14">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C14)*(Pricing!E:E=F14), 0))*E14</f>
@@ -1299,7 +1244,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G15" cm="1">
         <f t="array" ref="G15">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C15)*(Pricing!E:E=F15), 0))*E15</f>
@@ -1316,7 +1261,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G16" cm="1">
         <f t="array" ref="G16">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C16)*(Pricing!E:E=F16), 0))*E16</f>
@@ -1333,7 +1278,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" cm="1">
         <f t="array" ref="G17">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C17)*(Pricing!E:E=F17), 0))*E17</f>
@@ -1350,7 +1295,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18" cm="1">
         <f t="array" ref="G18">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C18)*(Pricing!E:E=F18), 0))*E18</f>
@@ -1367,7 +1312,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G19" cm="1">
         <f t="array" ref="G19">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C19)*(Pricing!E:E=F19), 0))*E19</f>
@@ -1384,7 +1329,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" cm="1">
         <f t="array" ref="G20">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C20)*(Pricing!E:E=F20), 0))*E20</f>
@@ -1401,7 +1346,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G21" cm="1">
         <f t="array" ref="G21">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C21)*(Pricing!E:E=F21), 0))*E21</f>
@@ -1418,7 +1363,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" cm="1">
         <f t="array" ref="G22">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C22)*(Pricing!E:E=F22), 0))*E22</f>
@@ -1435,7 +1380,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G23" cm="1">
         <f t="array" ref="G23">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C23)*(Pricing!E:E=F23), 0))*E23</f>
@@ -1452,7 +1397,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" cm="1">
         <f t="array" ref="G24">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C24)*(Pricing!E:E=F24), 0))*E24</f>
@@ -1469,7 +1414,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" cm="1">
         <f t="array" ref="G25">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C25)*(Pricing!E:E=F25), 0))*E25</f>
@@ -1486,7 +1431,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G26" cm="1">
         <f t="array" ref="G26">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C26)*(Pricing!E:E=F26), 0))*E26</f>
@@ -1503,7 +1448,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G27" cm="1">
         <f t="array" ref="G27">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C27)*(Pricing!E:E=F27), 0))*E27</f>
@@ -1520,7 +1465,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G28" cm="1">
         <f t="array" ref="G28">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C28)*(Pricing!E:E=F28), 0))*E28</f>
@@ -1537,7 +1482,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G29" cm="1">
         <f t="array" ref="G29">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C29)*(Pricing!E:E=F29), 0))*E29</f>
@@ -1554,28 +1499,11 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>24</v>
-      </c>
-      <c r="G30" cm="1">
-        <f t="array" ref="G30">INDEX(Pricing!G:G, MATCH(1,(Pricing!B:B=C30)*(Pricing!E:E=F30), 0))*E30</f>
-        <v>0</v>
-      </c>
-      <c r="H30" cm="1">
-        <f t="array" ref="H30">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C30)*(Pricing!E:E=F30), 0))*E30</f>
-        <v>0</v>
-      </c>
-      <c r="I30" cm="1">
-        <f t="array" ref="I30">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C30)*(Pricing!E:E=F30), 0))*E30</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
         <v>26</v>
       </c>
     </row>
@@ -1583,9 +1511,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1602,17 +1529,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
@@ -1644,168 +1571,132 @@
         <v>Asia Pacific (Singapore)</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <f>SUM(G6:G100)</f>
+        <v>3610.212</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4">
+        <f>SUM(H7:H100)</f>
+        <v>8938.4759999999987</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="str" cm="1">
-        <f t="array" ref="D5">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C5)*(Pricing!E:E=F5), 0))</f>
+      <c r="D7" t="str" cm="1">
+        <f t="array" ref="D7">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))</f>
         <v>Number of VPC</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F7" t="str">
         <f>$C$2</f>
         <v>ap-southeast-1</v>
       </c>
-      <c r="G5" cm="1">
-        <f t="array" ref="G5">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C5)*(Pricing!E:E=F5), 0))*E5</f>
-        <v>0</v>
-      </c>
-      <c r="H5" cm="1">
-        <f t="array" ref="H5">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C5)*(Pricing!E:E=F5), 0))*E5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="str" cm="1">
-        <f t="array" ref="D6">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))</f>
-        <v>Number of Instances</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:F9" si="0">$C$2</f>
-        <v>ap-southeast-1</v>
-      </c>
-      <c r="G6" cm="1">
-        <f t="array" ref="G6">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))*E6</f>
-        <v>1550.5199999999998</v>
-      </c>
-      <c r="H6" cm="1">
-        <f t="array" ref="H6">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C6)*(Pricing!E:E=F6), 0))*E6</f>
-        <v>4651.5599999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="str" cm="1">
-        <f t="array" ref="D7">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))</f>
-        <v>GB</v>
-      </c>
-      <c r="E7">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>ap-southeast-1</v>
-      </c>
       <c r="G7" cm="1">
         <f t="array" ref="G7">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))*E7</f>
-        <v>72.357599999999991</v>
+        <v>0</v>
       </c>
       <c r="H7" cm="1">
         <f t="array" ref="H7">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C7)*(Pricing!E:E=F7), 0))*E7</f>
-        <v>217.07280000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" ref="D8">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))</f>
-        <v>Number of Ips</v>
+        <v>Number of Instances</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F8:F11" si="0">$C$2</f>
         <v>ap-southeast-1</v>
       </c>
       <c r="G8" cm="1">
         <f t="array" ref="G8">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))*E8</f>
-        <v>175.20000000000002</v>
+        <v>1550.5199999999998</v>
       </c>
       <c r="H8" cm="1">
         <f t="array" ref="H8">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C8)*(Pricing!E:E=F8), 0))*E8</f>
-        <v>525.6</v>
+        <v>4651.5599999999995</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" ref="D9">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))</f>
-        <v>Number of Instances</v>
+        <v>GB month</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -1813,42 +1704,76 @@
       </c>
       <c r="G9" cm="1">
         <f t="array" ref="G9">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))*E9</f>
-        <v>1863.2520000000002</v>
+        <v>21.24</v>
       </c>
       <c r="H9" cm="1">
         <f t="array" ref="H9">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C9)*(Pricing!E:E=F9), 0))*E9</f>
-        <v>3697.5959999999995</v>
+        <v>63.719999999999992</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="str" cm="1">
+        <f t="array" ref="D10">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))</f>
+        <v>Number of Ips</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>ap-southeast-1</v>
       </c>
       <c r="G10" cm="1">
         <f t="array" ref="G10">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))*E10</f>
-        <v>0</v>
+        <v>175.20000000000002</v>
       </c>
       <c r="H10" cm="1">
         <f t="array" ref="H10">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C10)*(Pricing!E:E=F10), 0))*E10</f>
-        <v>0</v>
+        <v>525.6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="str" cm="1">
+        <f t="array" ref="D11">INDEX(Pricing!D:D, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))</f>
+        <v>Number of Instances</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>ap-southeast-1</v>
       </c>
       <c r="G11" cm="1">
         <f t="array" ref="G11">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))*E11</f>
-        <v>0</v>
+        <v>1863.2520000000002</v>
       </c>
       <c r="H11" cm="1">
         <f t="array" ref="H11">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C11)*(Pricing!E:E=F11), 0))*E11</f>
-        <v>0</v>
+        <v>3697.5959999999995</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G12" cm="1">
         <f t="array" ref="G12">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C12)*(Pricing!E:E=F12), 0))*E12</f>
@@ -1861,7 +1786,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G13" cm="1">
         <f t="array" ref="G13">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C13)*(Pricing!E:E=F13), 0))*E13</f>
@@ -1874,7 +1799,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14" cm="1">
         <f t="array" ref="G14">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C14)*(Pricing!E:E=F14), 0))*E14</f>
@@ -1887,7 +1812,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G15" cm="1">
         <f t="array" ref="G15">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C15)*(Pricing!E:E=F15), 0))*E15</f>
@@ -1900,7 +1825,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" cm="1">
         <f t="array" ref="G16">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C16)*(Pricing!E:E=F16), 0))*E16</f>
@@ -1913,7 +1838,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G17" cm="1">
         <f t="array" ref="G17">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C17)*(Pricing!E:E=F17), 0))*E17</f>
@@ -1926,7 +1851,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G18" cm="1">
         <f t="array" ref="G18">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C18)*(Pricing!E:E=F18), 0))*E18</f>
@@ -1939,7 +1864,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G19" cm="1">
         <f t="array" ref="G19">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C19)*(Pricing!E:E=F19), 0))*E19</f>
@@ -1952,7 +1877,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G20" cm="1">
         <f t="array" ref="G20">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C20)*(Pricing!E:E=F20), 0))*E20</f>
@@ -1965,7 +1890,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G21" cm="1">
         <f t="array" ref="G21">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C21)*(Pricing!E:E=F21), 0))*E21</f>
@@ -1978,7 +1903,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G22" cm="1">
         <f t="array" ref="G22">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C22)*(Pricing!E:E=F22), 0))*E22</f>
@@ -1991,7 +1916,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G23" cm="1">
         <f t="array" ref="G23">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C23)*(Pricing!E:E=F23), 0))*E23</f>
@@ -2004,7 +1929,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24" cm="1">
         <f t="array" ref="G24">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C24)*(Pricing!E:E=F24), 0))*E24</f>
@@ -2017,7 +1942,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G25" cm="1">
         <f t="array" ref="G25">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C25)*(Pricing!E:E=F25), 0))*E25</f>
@@ -2030,7 +1955,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G26" cm="1">
         <f t="array" ref="G26">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C26)*(Pricing!E:E=F26), 0))*E26</f>
@@ -2043,7 +1968,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G27" cm="1">
         <f t="array" ref="G27">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C27)*(Pricing!E:E=F27), 0))*E27</f>
@@ -2056,7 +1981,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G28" cm="1">
         <f t="array" ref="G28">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C28)*(Pricing!E:E=F28), 0))*E28</f>
@@ -2069,11 +1994,37 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="G29" cm="1">
+        <f t="array" ref="G29">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C29)*(Pricing!E:E=F29), 0))*E29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" cm="1">
+        <f t="array" ref="H29">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C29)*(Pricing!E:E=F29), 0))*E29</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="G30" cm="1">
+        <f t="array" ref="G30">INDEX(Pricing!H:H, MATCH(1,(Pricing!B:B=C30)*(Pricing!E:E=F30), 0))*E30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" cm="1">
+        <f t="array" ref="H30">INDEX(Pricing!I:I, MATCH(1,(Pricing!B:B=C30)*(Pricing!E:E=F30), 0))*E30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>26</v>
       </c>
     </row>
@@ -2082,7 +2033,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2106,7 +2056,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,16 +2134,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -2257,25 +2207,25 @@
         <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>0.059</f>
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="G5">
-        <f>Time.Units!$B$2*Pricing!F5</f>
-        <v>43.07</v>
-      </c>
       <c r="H5">
-        <f>Time.Units!B3*Pricing!F5</f>
-        <v>516.83999999999992</v>
+        <f>Time.Units!$B$5*G5</f>
+        <v>0.70799999999999996</v>
       </c>
       <c r="I5">
-        <f>Time.Units!$B$4*Pricing!F5</f>
-        <v>1550.52</v>
+        <f>Time.Units!$B$6*G5</f>
+        <v>2.1239999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2377,7 +2327,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2402,7 +2352,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,13 +2530,16 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="XEB1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2622,8 +2575,26 @@
         <v>26280</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6">
+        <f>3*B5</f>
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2647,156 +2618,156 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
         <v>71</v>
       </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
         <v>76</v>
       </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s">
-        <v>80</v>
-      </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
         <v>81</v>
       </c>
-      <c r="B13" t="s">
-        <v>82</v>
-      </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2804,208 +2775,208 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
         <v>87</v>
       </c>
-      <c r="B17" t="s">
-        <v>88</v>
-      </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
         <v>89</v>
       </c>
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
         <v>91</v>
       </c>
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
         <v>93</v>
       </c>
-      <c r="B20" t="s">
-        <v>94</v>
-      </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
         <v>95</v>
       </c>
-      <c r="B21" t="s">
-        <v>96</v>
-      </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
         <v>97</v>
       </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" t="s">
         <v>101</v>
       </c>
-      <c r="B24" t="s">
-        <v>102</v>
-      </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
         <v>103</v>
       </c>
-      <c r="B25" t="s">
-        <v>104</v>
-      </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
         <v>105</v>
       </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
         <v>107</v>
       </c>
-      <c r="B27" t="s">
-        <v>108</v>
-      </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
         <v>109</v>
       </c>
-      <c r="B28" t="s">
-        <v>110</v>
-      </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
         <v>111</v>
       </c>
-      <c r="B29" t="s">
-        <v>112</v>
-      </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" t="s">
         <v>113</v>
       </c>
-      <c r="B30" t="s">
-        <v>114</v>
-      </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" t="s">
         <v>115</v>
       </c>
-      <c r="B31" t="s">
-        <v>116</v>
-      </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
         <v>117</v>
       </c>
-      <c r="B32" t="s">
-        <v>118</v>
-      </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" t="s">
         <v>119</v>
       </c>
-      <c r="B33" t="s">
-        <v>120</v>
-      </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>